<commit_message>
Final Draft Vehicle SSPs
</commit_message>
<xml_diff>
--- a/Client Service Framework/OSMS_Orchestration.xlsx
+++ b/Client Service Framework/OSMS_Orchestration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="660" windowWidth="30760" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-28220" yWindow="1720" windowWidth="30760" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -931,7 +931,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>